<commit_message>
Add: Script Fusion, README e outros itens
</commit_message>
<xml_diff>
--- a/banco_de_massas.xlsx
+++ b/banco_de_massas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeltaV\Documents\Eliton Sena de Souza\CM-Calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F35783-7BC5-4AC6-8776-1AD3E4C5E356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD5CB75-9F8B-4DCD-9D9A-822D83430AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
     <t>ChavetaDir:1</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Topo</t>
   </si>
   <si>
-    <t>Massa</t>
-  </si>
-  <si>
     <t>Fix RC</t>
   </si>
   <si>
@@ -156,6 +150,12 @@
   </si>
   <si>
     <t>Voltímetro:1</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>massa</t>
   </si>
 </sst>
 </file>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,15 +557,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>66.957366239999999</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>66.957366239999999</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>18.7</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1">
         <v>504.4</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1">
         <v>0.1</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>0.1</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>0.23902363999999998</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>0.23902363999999998</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>0.23902363999999998</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>0.23902363999999998</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1">
         <v>0.56000000000000005</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1">
         <v>0.56000000000000005</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1">
         <v>6.1</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>5.3</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1">
         <v>6.9</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
         <v>6.1</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1">
         <v>0.9</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1">
         <v>0.9</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1">
         <v>3.3</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1">
         <v>5.6</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1">
         <v>4.3</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2">
         <v>995</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
         <v>39.4</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1">
         <v>20.440000000000001</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1">
         <v>3.75</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1">
         <v>3.75</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1">
         <v>10.8</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="1">
         <v>177.4</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1">
         <v>40.700000000000003</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1">
         <v>13.7</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="1">
         <v>50</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1">
         <v>4.5</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1">
         <v>20.75</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
         <v>145.47809828000001</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="1">
         <v>6.63</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1">
         <v>5.4</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="1">
         <v>26.5</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1">
         <v>15.48</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1">
         <v>11.4</v>

</xml_diff>